<commit_message>
Update test cases for LabCourse class testing.
</commit_message>
<xml_diff>
--- a/tests/M02_demonstration_test_plan_lab_course.xlsx
+++ b/tests/M02_demonstration_test_plan_lab_course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\3. Demonstrations\module_1\requirements_document\given_files\isd_demonstration\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daltenburg\source\repos\isd-demo-prep\comp-2327-fa2024-ft3\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A80CDF7-C4F7-4A4F-B73A-CB1201DFC192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DB69F8-4C82-4075-B09C-199FC1595593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -240,6 +240,57 @@
   </si>
   <si>
     <t>Lab Course</t>
+  </si>
+  <si>
+    <t>Damien Altenburg</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Object initialized with the correct state</t>
+  </si>
+  <si>
+    <t>Object initialized with the correct state (lab_equipment = "None")</t>
+  </si>
+  <si>
+    <t>Course: ISD
+Department: Computer Science
+Credit Hours: 90
+Lab Equipment: Laptop</t>
+  </si>
+  <si>
+    <t>Student(student_number = 123, name  = "Joe Smith", department = Department.COMPUTER_SCIENCE)</t>
+  </si>
+  <si>
+    <t>"Joe Smith has been successfully enrolled in ISD."</t>
+  </si>
+  <si>
+    <t>"Joe Smith has NOT been enrolled in lab: ISD due to insufficient capacity."</t>
+  </si>
+  <si>
+    <t>name = "ISD"
+department = Department.COMPUTER_SCIENCE
+credit_hours = 90
+capacity = 30
+current_enrollment = 14
+lab_eqiupment = "Laptop"</t>
+  </si>
+  <si>
+    <t>name = "ISD"
+department = Department.COMPUTER_SCIENCE
+credit_hours = 90
+capacity = 30
+current_enrollment = 14
+lab_eqiupment = ""</t>
+  </si>
+  <si>
+    <t>name = "ISD"
+department = Department.COMPUTER_SCIENCE
+credit_hours = 90
+capacity = 15
+current_enrollment = 15
+lab_eqiupment = "Laptop"</t>
   </si>
 </sst>
 </file>
@@ -1100,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,9 +1160,9 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" customWidth="1"/>
+    <col min="7" max="7" width="56.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1182,9 @@
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1166,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1177,11 +1230,17 @@
       <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1192,11 +1251,17 @@
       <c r="D8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>3</v>
       </c>
@@ -1206,11 +1271,17 @@
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
         <v>4</v>
       </c>
@@ -1220,11 +1291,17 @@
       <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>5</v>
       </c>
@@ -1234,9 +1311,15 @@
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="E11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12">

</xml_diff>